<commit_message>
add swapped anchors and 011520 results
</commit_message>
<xml_diff>
--- a/Simulation Results 011220 (wd=0.00001).xlsx
+++ b/Simulation Results 011220 (wd=0.00001).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BrianLam/UTSC Research/Plaut_Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A543744-6F71-5A46-9C38-4074A4A758D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5C9217-5694-6347-B52A-A9906C3937F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19080" activeTab="2" xr2:uid="{731A8A60-4D85-694D-9B57-3EC626427640}"/>
   </bookViews>
@@ -244,8 +244,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="119532" y="10443881"/>
-          <a:ext cx="5486400" cy="3657600"/>
+          <a:off x="119532" y="10021615"/>
+          <a:ext cx="5545098" cy="3430280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -345,15 +345,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>791884</xdr:colOff>
+      <xdr:colOff>819695</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>119528</xdr:rowOff>
+      <xdr:rowOff>147338</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>525931</xdr:colOff>
+      <xdr:colOff>553742</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>11952</xdr:rowOff>
+      <xdr:rowOff>39762</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -376,8 +376,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5722472" y="6603999"/>
-          <a:ext cx="5486400" cy="3657600"/>
+          <a:off x="5769914" y="6543688"/>
+          <a:ext cx="5509302" cy="3563373"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1402,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91334DBB-3320-CA41-8063-97F176F4831A}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="185" workbookViewId="0">
-      <selection activeCell="Q53" sqref="Q53"/>
+    <sheetView topLeftCell="A37" zoomScale="164" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1491,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A30168-F67C-BC4E-A581-6173ACDBEC56}">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="75" workbookViewId="0">
-      <selection activeCell="P63" sqref="P63"/>
+    <sheetView topLeftCell="A56" zoomScale="142" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45:H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1586,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED88E278-0A57-1441-9931-94C815493842}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="P52" sqref="P52"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="217" zoomScaleNormal="217" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>